<commit_message>
Iteration2: All documents. Steps towards It3
</commit_message>
<xml_diff>
--- a/Iteration2/After Coding/defect_log-Iteration2.xlsx
+++ b/Iteration2/After Coding/defect_log-Iteration2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nil0310\OneDrive - Ara Institute of Canterbury\Year 2\Semester 1\Software Engineering\Assignment 1\Iteration1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\OneDrive - Ara Institute of Canterbury\Year 2\Semester 1\Software Engineering\Assignment 1\Iteration2\After Coding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="11_9772094146B369BB7D2AB030540DAC71AB463A6C" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{5A4A1517-9980-4EE8-9427-227F73C1B186}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E82677-1252-4C2F-A7C2-B19BF8E02C6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="79">
   <si>
     <t>PSP Defect Recording Log</t>
   </si>
@@ -623,6 +623,21 @@
   </si>
   <si>
     <t>Compile</t>
+  </si>
+  <si>
+    <t>&lt;&gt; wrong way round</t>
+  </si>
+  <si>
+    <t>User could input number less than 1. Changed all numbers less than 1 to be 1</t>
+  </si>
+  <si>
+    <t>Error in v-on handler: "TypeError: Cannot read property 'getRandomNum' of undefined" in pickGameNumber(). -1 added to fix this</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Error in v-on handler: "TypeError: Cannot read property 'getRandomNum' of undefined" in getCalcGuess(). Fixed by putting -1 on array</t>
+  </si>
+  <si>
+    <t>Data/state remained the same for all games. Added reset function to clear data/state</t>
   </si>
 </sst>
 </file>
@@ -1282,7 +1297,7 @@
   <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1480,19 +1495,134 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H13" s="6"/>
+      <c r="A12" s="18">
+        <v>43567</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>6</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="18">
+        <v>43567</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>7</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H16" s="6"/>
+      <c r="A14" s="18">
+        <v>43567</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>60</v>
+      </c>
+      <c r="D14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>8</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="18">
+        <v>43567</v>
+      </c>
+      <c r="B15">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>9</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="18">
+        <v>43567</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>70</v>
+      </c>
+      <c r="D16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>10</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="17" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H17" s="6"/>

</xml_diff>